<commit_message>
Added electricity consumption profile generator. Variable appliances still need to be added.
</commit_message>
<xml_diff>
--- a/Material Database.xlsx
+++ b/Material Database.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\PHPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F88D9174-8435-4D59-ADC0-59284F277785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40422A1B-287A-4F9B-9137-403DFB4201A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8B72D96C-E835-4E6C-85A9-680D0CEA1045}"/>
+    <workbookView minimized="1" xWindow="7200" yWindow="6150" windowWidth="14940" windowHeight="7740" activeTab="1" xr2:uid="{8B72D96C-E835-4E6C-85A9-680D0CEA1045}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Materials" sheetId="1" r:id="rId1"/>
+    <sheet name="Inputs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -464,12 +465,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD98F7B-0D99-43C0-AD66-FCCE97E0ADD8}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
@@ -734,4 +736,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6A4828-4FE8-4409-A78E-CBF87BB23062}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>